<commit_message>
Atualizei a planilha KITS.xlsx
</commit_message>
<xml_diff>
--- a/KITS.xlsx
+++ b/KITS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doug\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Doug\Desktop\git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E2C0171-E614-4B62-AC97-B6CE9AA3FF65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABA4DE65-6CDF-43A2-9806-43C1C4CF4421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,7 +141,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="248">
   <si>
     <t>E-mail</t>
   </si>
@@ -174,9 +174,6 @@
   </si>
   <si>
     <t xml:space="preserve">Juliano </t>
-  </si>
-  <si>
-    <t>-</t>
   </si>
   <si>
     <t xml:space="preserve">Juliano Gonçalves </t>
@@ -534,9 +531,6 @@
     <t>José Geraldo de Araújo Silva</t>
   </si>
   <si>
-    <t>31 9 8751 3823</t>
-  </si>
-  <si>
     <t>UA3571037</t>
   </si>
   <si>
@@ -663,9 +657,6 @@
     <t>Emidio Oliveira Teixeira</t>
   </si>
   <si>
-    <t>38 991265463</t>
-  </si>
-  <si>
     <t>Judite Oliveira Teixeira</t>
   </si>
   <si>
@@ -708,9 +699,6 @@
     <t>Bianca Aparecida dos Santos Mello</t>
   </si>
   <si>
-    <t>18 996342066</t>
-  </si>
-  <si>
     <t>João dos Santos</t>
   </si>
   <si>
@@ -724,9 +712,6 @@
   </si>
   <si>
     <t>Laurita Martins de Oliveira</t>
-  </si>
-  <si>
-    <t>19 99690952</t>
   </si>
   <si>
     <t>Edileia Lopes Ramalho</t>
@@ -938,8 +923,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1163,14 +1151,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="30.5546875" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="86.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.109375" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="63.44140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6.6640625" bestFit="1" customWidth="1"/>
@@ -1188,11 +1176,11 @@
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -1220,32 +1208,29 @@
       <c r="B2" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>13</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>15</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" t="s">
         <v>16</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>17</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>18</v>
-      </c>
-      <c r="L2" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
@@ -1253,28 +1238,25 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>21</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -1282,28 +1264,25 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" t="s">
         <v>26</v>
       </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>27</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
         <v>28</v>
       </c>
-      <c r="F4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="J4" t="s">
         <v>29</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>30</v>
-      </c>
-      <c r="K4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1311,25 +1290,22 @@
         <v>9</v>
       </c>
       <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
         <v>34</v>
       </c>
-      <c r="F5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>35</v>
-      </c>
       <c r="J5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -1337,1264 +1313,1261 @@
         <v>9</v>
       </c>
       <c r="B6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" t="s">
         <v>36</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>37</v>
       </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
       <c r="F6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>40</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>41</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>42</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>43</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>44</v>
       </c>
-      <c r="H7" t="s">
+      <c r="J7" t="s">
         <v>45</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>46</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>47</v>
-      </c>
-      <c r="L7" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
         <v>49</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="1">
+        <v>11997003120</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
         <v>50</v>
       </c>
-      <c r="C8">
-        <v>11997003120</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-      <c r="E8" t="s">
+      <c r="H8" t="s">
         <v>51</v>
       </c>
-      <c r="H8" t="s">
+      <c r="K8" t="s">
         <v>52</v>
-      </c>
-      <c r="K8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="1">
+        <v>11997003120</v>
+      </c>
+      <c r="D9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E9" t="s">
         <v>54</v>
       </c>
-      <c r="C9">
-        <v>11997003120</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" t="s">
-        <v>55</v>
-      </c>
       <c r="H9" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" t="s">
         <v>52</v>
-      </c>
-      <c r="K9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C10" s="1">
+        <v>11997003120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
         <v>56</v>
       </c>
-      <c r="C10">
-        <v>11997003120</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="H10" t="s">
         <v>57</v>
       </c>
-      <c r="H10" t="s">
-        <v>58</v>
-      </c>
       <c r="K10" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" s="1">
+        <v>11997003120</v>
+      </c>
+      <c r="D11" t="s">
+        <v>58</v>
+      </c>
+      <c r="E11" t="s">
         <v>59</v>
       </c>
-      <c r="C11">
-        <v>11997003120</v>
-      </c>
-      <c r="D11" t="s">
-        <v>59</v>
-      </c>
-      <c r="E11" t="s">
+      <c r="H11" t="s">
         <v>60</v>
       </c>
-      <c r="H11" t="s">
-        <v>61</v>
-      </c>
       <c r="K11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" t="s">
         <v>62</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" s="1">
+        <v>31999116100</v>
+      </c>
+      <c r="D12" t="s">
+        <v>62</v>
+      </c>
+      <c r="E12" t="s">
         <v>63</v>
       </c>
-      <c r="C12">
-        <v>31999116100</v>
-      </c>
-      <c r="D12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>64</v>
       </c>
-      <c r="F12" t="s">
+      <c r="J12" t="s">
         <v>65</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>66</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>67</v>
-      </c>
-      <c r="L12" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" t="s">
         <v>62</v>
       </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13">
+      <c r="C13" s="1">
         <v>31999116100</v>
       </c>
       <c r="D13" t="s">
+        <v>68</v>
+      </c>
+      <c r="E13" t="s">
         <v>69</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G13" t="s">
         <v>70</v>
       </c>
-      <c r="F13" t="s">
+      <c r="J13" t="s">
         <v>65</v>
       </c>
-      <c r="G13" t="s">
+      <c r="K13" t="s">
         <v>71</v>
-      </c>
-      <c r="J13" t="s">
-        <v>66</v>
-      </c>
-      <c r="K13" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" t="s">
         <v>62</v>
       </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14">
+      <c r="C14" s="1">
         <v>31999116100</v>
       </c>
       <c r="D14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E14" t="s">
         <v>73</v>
       </c>
-      <c r="E14" t="s">
-        <v>74</v>
-      </c>
       <c r="F14" t="s">
+        <v>64</v>
+      </c>
+      <c r="J14" t="s">
         <v>65</v>
-      </c>
-      <c r="J14" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" t="s">
         <v>62</v>
       </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>31999116100</v>
       </c>
       <c r="D15" t="s">
+        <v>74</v>
+      </c>
+      <c r="E15" t="s">
         <v>75</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>76</v>
       </c>
-      <c r="F15" t="s">
-        <v>77</v>
-      </c>
       <c r="J15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" t="s">
         <v>78</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" s="1">
+        <v>61999648406</v>
+      </c>
+      <c r="D16" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" t="s">
         <v>79</v>
-      </c>
-      <c r="C16">
-        <v>61999648406</v>
-      </c>
-      <c r="D16" t="s">
-        <v>79</v>
-      </c>
-      <c r="E16" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
         <v>81</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" s="1">
+        <v>31994073371</v>
+      </c>
+      <c r="H17" t="s">
         <v>82</v>
       </c>
-      <c r="C17">
-        <v>31994073371</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="J17" t="s">
         <v>83</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>84</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>85</v>
-      </c>
-      <c r="L17" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25"/>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" t="s">
         <v>87</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" s="1">
+        <v>491629473668</v>
+      </c>
+      <c r="D19" t="s">
+        <v>87</v>
+      </c>
+      <c r="E19" t="s">
         <v>88</v>
       </c>
-      <c r="C19">
-        <f t="shared" ref="C19:C21" si="0">491629473668</f>
-        <v>491629473668</v>
-      </c>
-      <c r="D19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="J19" t="s">
+        <v>83</v>
+      </c>
+      <c r="K19" t="s">
         <v>89</v>
       </c>
-      <c r="J19" t="s">
-        <v>84</v>
-      </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>90</v>
-      </c>
-      <c r="L19" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B20" t="s">
         <v>87</v>
       </c>
-      <c r="B20" t="s">
-        <v>88</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="0"/>
+      <c r="C20" s="1">
         <v>491629473668</v>
       </c>
       <c r="D20" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" t="s">
         <v>92</v>
       </c>
-      <c r="E20" t="s">
-        <v>93</v>
-      </c>
       <c r="J20" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K20" t="s">
+        <v>89</v>
+      </c>
+      <c r="L20" t="s">
         <v>90</v>
-      </c>
-      <c r="L20" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B21" t="s">
+        <v>93</v>
+      </c>
+      <c r="C21" s="1">
+        <v>491629473668</v>
+      </c>
+      <c r="D21" t="s">
         <v>94</v>
       </c>
-      <c r="C21">
-        <f t="shared" si="0"/>
-        <v>491629473668</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>95</v>
       </c>
-      <c r="E21" t="s">
-        <v>96</v>
-      </c>
       <c r="J21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K21" t="s">
+        <v>89</v>
+      </c>
+      <c r="L21" t="s">
         <v>90</v>
-      </c>
-      <c r="L21" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" t="s">
         <v>97</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" s="1">
+        <v>11981038105</v>
+      </c>
+      <c r="E22" t="s">
         <v>98</v>
       </c>
-      <c r="C22">
-        <v>11981038105</v>
-      </c>
-      <c r="E22" t="s">
+      <c r="G22" t="s">
         <v>99</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>100</v>
       </c>
-      <c r="H22" t="s">
+      <c r="J22" t="s">
+        <v>83</v>
+      </c>
+      <c r="K22" t="s">
         <v>101</v>
       </c>
-      <c r="J22" t="s">
-        <v>84</v>
-      </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>102</v>
-      </c>
-      <c r="L22" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B23" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="1">
+        <v>11981038105</v>
+      </c>
+      <c r="D23" t="s">
         <v>104</v>
       </c>
-      <c r="C23">
-        <v>11981038105</v>
-      </c>
-      <c r="D23" t="s">
+      <c r="E23" t="s">
         <v>105</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>106</v>
       </c>
-      <c r="F23" t="s">
+      <c r="H23" t="s">
         <v>107</v>
       </c>
-      <c r="H23" t="s">
-        <v>108</v>
-      </c>
       <c r="J23" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K23" t="s">
+        <v>101</v>
+      </c>
+      <c r="L23" t="s">
         <v>102</v>
-      </c>
-      <c r="L23" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B24" t="s">
+        <v>108</v>
+      </c>
+      <c r="C24" s="1">
+        <v>11981038105</v>
+      </c>
+      <c r="D24" t="s">
+        <v>104</v>
+      </c>
+      <c r="E24" t="s">
         <v>109</v>
       </c>
-      <c r="C24">
-        <v>11981038105</v>
-      </c>
-      <c r="D24" t="s">
-        <v>105</v>
-      </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>110</v>
       </c>
-      <c r="F24" t="s">
+      <c r="H24" t="s">
         <v>111</v>
       </c>
-      <c r="H24" t="s">
+      <c r="J24" t="s">
+        <v>83</v>
+      </c>
+      <c r="K24" t="s">
+        <v>101</v>
+      </c>
+      <c r="L24" t="s">
         <v>112</v>
-      </c>
-      <c r="J24" t="s">
-        <v>84</v>
-      </c>
-      <c r="K24" t="s">
-        <v>102</v>
-      </c>
-      <c r="L24" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B25" t="s">
+        <v>113</v>
+      </c>
+      <c r="C25" s="1">
+        <v>11981038105</v>
+      </c>
+      <c r="D25" t="s">
+        <v>104</v>
+      </c>
+      <c r="E25" t="s">
         <v>114</v>
       </c>
-      <c r="C25">
-        <v>11981038105</v>
-      </c>
-      <c r="D25" t="s">
-        <v>105</v>
-      </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" t="s">
+        <v>99</v>
+      </c>
+      <c r="H25" t="s">
         <v>115</v>
       </c>
-      <c r="F25" t="s">
-        <v>107</v>
-      </c>
-      <c r="G25" t="s">
-        <v>100</v>
-      </c>
-      <c r="H25" t="s">
-        <v>116</v>
-      </c>
       <c r="J25" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K25" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="L25" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B26" t="s">
+        <v>116</v>
+      </c>
+      <c r="C26" s="1">
+        <v>11981038105</v>
+      </c>
+      <c r="D26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" t="s">
         <v>117</v>
       </c>
-      <c r="C26">
-        <v>11981038105</v>
-      </c>
-      <c r="D26" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" t="s">
-        <v>118</v>
-      </c>
       <c r="G26" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B27" t="s">
-        <v>105</v>
-      </c>
-      <c r="C27">
+        <v>104</v>
+      </c>
+      <c r="C27" s="1">
         <v>11981038105</v>
       </c>
       <c r="D27" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E27" t="s">
+        <v>118</v>
+      </c>
+      <c r="F27" t="s">
         <v>119</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
+        <v>99</v>
+      </c>
+      <c r="H27" t="s">
         <v>120</v>
       </c>
-      <c r="G27" t="s">
-        <v>100</v>
-      </c>
-      <c r="H27" t="s">
-        <v>121</v>
-      </c>
       <c r="J27" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K27" t="s">
+        <v>101</v>
+      </c>
+      <c r="L27" t="s">
         <v>102</v>
-      </c>
-      <c r="L27" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>121</v>
+      </c>
+      <c r="B28" t="s">
         <v>122</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" s="1">
+        <v>33988937861</v>
+      </c>
+      <c r="D28" t="s">
         <v>123</v>
       </c>
-      <c r="C28">
-        <v>33988937861</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="E28" t="s">
         <v>124</v>
-      </c>
-      <c r="E28" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>126</v>
+      </c>
+      <c r="B30" t="s">
         <v>127</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" s="1">
+        <v>31987513823</v>
+      </c>
+      <c r="D30" t="s">
+        <v>127</v>
+      </c>
+      <c r="E30" t="s">
         <v>128</v>
-      </c>
-      <c r="C30" t="s">
-        <v>129</v>
-      </c>
-      <c r="D30" t="s">
-        <v>128</v>
-      </c>
-      <c r="E30" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B31" t="s">
         <v>127</v>
       </c>
-      <c r="B31" t="s">
-        <v>128</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1">
+        <v>31987513823</v>
+      </c>
+      <c r="D31" t="s">
         <v>129</v>
       </c>
-      <c r="D31" t="s">
-        <v>131</v>
-      </c>
       <c r="E31" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>126</v>
+      </c>
+      <c r="B32" t="s">
         <v>127</v>
       </c>
-      <c r="B32" t="s">
-        <v>128</v>
-      </c>
-      <c r="C32" t="s">
-        <v>129</v>
+      <c r="C32" s="1">
+        <v>31987513823</v>
       </c>
       <c r="D32" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E32" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>126</v>
+      </c>
+      <c r="B33" t="s">
         <v>127</v>
       </c>
-      <c r="B33" t="s">
-        <v>128</v>
-      </c>
-      <c r="C33" t="s">
-        <v>129</v>
+      <c r="C33" s="1">
+        <v>31987513823</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E33" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>126</v>
+      </c>
+      <c r="B34" t="s">
         <v>127</v>
       </c>
-      <c r="B34" t="s">
-        <v>128</v>
-      </c>
-      <c r="C34" t="s">
-        <v>129</v>
+      <c r="C34" s="1">
+        <v>31987513823</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>126</v>
+      </c>
+      <c r="B35" t="s">
         <v>127</v>
       </c>
-      <c r="B35" t="s">
-        <v>128</v>
-      </c>
-      <c r="C35" t="s">
-        <v>129</v>
+      <c r="C35" s="1">
+        <v>31987513823</v>
       </c>
       <c r="D35" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E35" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
+        <v>126</v>
+      </c>
+      <c r="B36" t="s">
         <v>127</v>
       </c>
-      <c r="B36" t="s">
-        <v>128</v>
-      </c>
-      <c r="C36" t="s">
-        <v>129</v>
+      <c r="C36" s="1">
+        <v>31987513823</v>
       </c>
       <c r="D36" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E36" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" t="s">
         <v>127</v>
       </c>
-      <c r="B37" t="s">
-        <v>128</v>
-      </c>
-      <c r="C37" t="s">
-        <v>129</v>
+      <c r="C37" s="1">
+        <v>31987513823</v>
       </c>
       <c r="D37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E37" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>126</v>
+      </c>
+      <c r="B38" t="s">
         <v>127</v>
       </c>
-      <c r="B38" t="s">
-        <v>128</v>
-      </c>
-      <c r="C38" t="s">
-        <v>129</v>
+      <c r="C38" s="1">
+        <v>31987513823</v>
       </c>
       <c r="D38" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>126</v>
+      </c>
+      <c r="B39" t="s">
         <v>127</v>
       </c>
-      <c r="B39" t="s">
-        <v>128</v>
-      </c>
-      <c r="C39" t="s">
-        <v>129</v>
+      <c r="C39" s="1">
+        <v>31987513823</v>
       </c>
       <c r="D39" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E39" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>126</v>
+      </c>
+      <c r="B40" t="s">
         <v>127</v>
       </c>
-      <c r="B40" t="s">
-        <v>128</v>
-      </c>
-      <c r="C40" t="s">
-        <v>129</v>
+      <c r="C40" s="1">
+        <v>31987513823</v>
       </c>
       <c r="D40" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E40" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>126</v>
+      </c>
+      <c r="B41" t="s">
         <v>127</v>
       </c>
-      <c r="B41" t="s">
-        <v>128</v>
-      </c>
-      <c r="C41" t="s">
-        <v>129</v>
+      <c r="C41" s="1">
+        <v>31987513823</v>
       </c>
       <c r="D41" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E41" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>151</v>
+      </c>
+      <c r="B42" t="s">
+        <v>152</v>
+      </c>
+      <c r="C42" s="1">
+        <v>61993281839</v>
+      </c>
+      <c r="D42" t="s">
         <v>153</v>
       </c>
-      <c r="B42" t="s">
+      <c r="E42" t="s">
         <v>154</v>
-      </c>
-      <c r="C42">
-        <v>61993281839</v>
-      </c>
-      <c r="D42" t="s">
-        <v>155</v>
-      </c>
-      <c r="E42" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
+        <v>155</v>
+      </c>
+      <c r="B44" t="s">
+        <v>156</v>
+      </c>
+      <c r="D44" t="s">
+        <v>156</v>
+      </c>
+      <c r="E44" t="s">
         <v>157</v>
       </c>
-      <c r="B44" t="s">
+      <c r="H44" t="s">
         <v>158</v>
       </c>
-      <c r="D44" t="s">
-        <v>158</v>
-      </c>
-      <c r="E44" t="s">
+      <c r="K44" t="s">
         <v>159</v>
       </c>
-      <c r="H44" t="s">
+      <c r="L44" t="s">
         <v>160</v>
-      </c>
-      <c r="K44" t="s">
-        <v>161</v>
-      </c>
-      <c r="L44" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>161</v>
+      </c>
+      <c r="B45" t="s">
+        <v>162</v>
+      </c>
+      <c r="C45" s="1">
+        <v>14991294599</v>
+      </c>
+      <c r="D45" t="s">
+        <v>162</v>
+      </c>
+      <c r="E45" t="s">
         <v>163</v>
       </c>
-      <c r="B45" t="s">
+      <c r="F45" t="s">
         <v>164</v>
       </c>
-      <c r="C45">
-        <v>14991294599</v>
-      </c>
-      <c r="D45" t="s">
-        <v>164</v>
-      </c>
-      <c r="E45" t="s">
+      <c r="G45" t="s">
         <v>165</v>
       </c>
-      <c r="F45" t="s">
+      <c r="H45" t="s">
         <v>166</v>
       </c>
-      <c r="G45" t="s">
+      <c r="L45" t="s">
         <v>167</v>
-      </c>
-      <c r="H45" t="s">
-        <v>168</v>
-      </c>
-      <c r="L45" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>168</v>
+      </c>
+      <c r="B46" t="s">
+        <v>169</v>
+      </c>
+      <c r="C46" s="1">
+        <v>38991265463</v>
+      </c>
+      <c r="D46" t="s">
         <v>170</v>
       </c>
-      <c r="B46" t="s">
+      <c r="E46" t="s">
         <v>171</v>
       </c>
-      <c r="C46" t="s">
+      <c r="F46" t="s">
+        <v>76</v>
+      </c>
+      <c r="H46" t="s">
         <v>172</v>
       </c>
-      <c r="D46" t="s">
+      <c r="K46" t="s">
         <v>173</v>
-      </c>
-      <c r="E46" t="s">
-        <v>174</v>
-      </c>
-      <c r="F46" t="s">
-        <v>77</v>
-      </c>
-      <c r="H46" t="s">
-        <v>175</v>
-      </c>
-      <c r="K46" t="s">
-        <v>176</v>
       </c>
     </row>
     <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B47" t="s">
-        <v>171</v>
-      </c>
-      <c r="C47" t="s">
-        <v>172</v>
+        <v>169</v>
+      </c>
+      <c r="C47" s="1">
+        <v>38991265463</v>
       </c>
       <c r="D47" t="s">
+        <v>174</v>
+      </c>
+      <c r="E47" t="s">
+        <v>175</v>
+      </c>
+      <c r="F47" t="s">
+        <v>76</v>
+      </c>
+      <c r="H47" t="s">
+        <v>176</v>
+      </c>
+      <c r="K47" t="s">
         <v>177</v>
       </c>
-      <c r="E47" t="s">
+      <c r="L47" t="s">
         <v>178</v>
-      </c>
-      <c r="F47" t="s">
-        <v>77</v>
-      </c>
-      <c r="H47" t="s">
-        <v>179</v>
-      </c>
-      <c r="K47" t="s">
-        <v>180</v>
-      </c>
-      <c r="L47" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B48" t="s">
-        <v>183</v>
-      </c>
-      <c r="C48">
+        <v>180</v>
+      </c>
+      <c r="C48" s="1">
         <v>37991529959</v>
       </c>
       <c r="E48" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>182</v>
+      </c>
+      <c r="B49" t="s">
+        <v>183</v>
+      </c>
+      <c r="C49" s="1">
+        <v>18996342066</v>
+      </c>
+      <c r="D49" t="s">
+        <v>184</v>
+      </c>
+      <c r="E49" t="s">
         <v>185</v>
       </c>
-      <c r="B49" t="s">
+      <c r="H49" t="s">
         <v>186</v>
-      </c>
-      <c r="C49" t="s">
-        <v>187</v>
-      </c>
-      <c r="D49" t="s">
-        <v>188</v>
-      </c>
-      <c r="E49" t="s">
-        <v>189</v>
-      </c>
-      <c r="H49" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
+        <v>187</v>
+      </c>
+      <c r="B50" t="s">
+        <v>188</v>
+      </c>
+      <c r="C50" s="1">
+        <v>1999690952</v>
+      </c>
+      <c r="D50" t="s">
+        <v>189</v>
+      </c>
+      <c r="E50" t="s">
+        <v>190</v>
+      </c>
+      <c r="H50" t="s">
         <v>191</v>
-      </c>
-      <c r="B50" t="s">
-        <v>192</v>
-      </c>
-      <c r="C50" t="s">
-        <v>193</v>
-      </c>
-      <c r="D50" t="s">
-        <v>194</v>
-      </c>
-      <c r="E50" t="s">
-        <v>195</v>
-      </c>
-      <c r="H50" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B51" t="s">
-        <v>171</v>
-      </c>
-      <c r="C51" t="s">
-        <v>172</v>
+        <v>169</v>
+      </c>
+      <c r="C51" s="1">
+        <v>38991265463</v>
       </c>
       <c r="D51" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E51" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="F51" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="G51" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H51" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B52" t="s">
-        <v>171</v>
-      </c>
-      <c r="C52" t="s">
-        <v>172</v>
+        <v>169</v>
+      </c>
+      <c r="C52" s="1">
+        <v>38991265463</v>
       </c>
       <c r="D52" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E52" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="F52" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="H52" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B53" t="s">
-        <v>171</v>
-      </c>
-      <c r="C53" t="s">
+        <v>169</v>
+      </c>
+      <c r="C53" s="1">
+        <v>38991265463</v>
+      </c>
+      <c r="D53" t="s">
+        <v>198</v>
+      </c>
+      <c r="E53" t="s">
+        <v>199</v>
+      </c>
+      <c r="F53" t="s">
+        <v>200</v>
+      </c>
+      <c r="G53" t="s">
+        <v>165</v>
+      </c>
+      <c r="H53" t="s">
         <v>172</v>
-      </c>
-      <c r="D53" t="s">
-        <v>203</v>
-      </c>
-      <c r="E53" t="s">
-        <v>204</v>
-      </c>
-      <c r="F53" t="s">
-        <v>205</v>
-      </c>
-      <c r="G53" t="s">
-        <v>167</v>
-      </c>
-      <c r="H53" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B54" t="s">
-        <v>171</v>
-      </c>
-      <c r="C54" t="s">
-        <v>172</v>
+        <v>169</v>
+      </c>
+      <c r="C54" s="1">
+        <v>38991265463</v>
       </c>
       <c r="D54" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E54" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="F54" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="H54" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B55" t="s">
-        <v>164</v>
-      </c>
-      <c r="C55">
+        <v>162</v>
+      </c>
+      <c r="C55" s="1">
         <v>14991294599</v>
       </c>
       <c r="D55" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E55" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="F55" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G55" t="s">
+        <v>165</v>
+      </c>
+      <c r="H55" t="s">
+        <v>206</v>
+      </c>
+      <c r="L55" t="s">
         <v>167</v>
-      </c>
-      <c r="H55" t="s">
-        <v>211</v>
-      </c>
-      <c r="L55" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>207</v>
+      </c>
+      <c r="B56" t="s">
+        <v>208</v>
+      </c>
+      <c r="C56" s="1">
+        <v>34639507559</v>
+      </c>
+      <c r="D56" t="s">
+        <v>209</v>
+      </c>
+      <c r="E56" t="s">
+        <v>210</v>
+      </c>
+      <c r="F56" t="s">
+        <v>211</v>
+      </c>
+      <c r="H56" t="s">
         <v>212</v>
       </c>
-      <c r="B56" t="s">
+      <c r="L56" t="s">
         <v>213</v>
-      </c>
-      <c r="C56">
-        <v>34639507559</v>
-      </c>
-      <c r="D56" t="s">
-        <v>214</v>
-      </c>
-      <c r="E56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F56" t="s">
-        <v>216</v>
-      </c>
-      <c r="H56" t="s">
-        <v>217</v>
-      </c>
-      <c r="L56" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E57" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
     </row>
     <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="B58" t="s">
-        <v>221</v>
-      </c>
-      <c r="C58">
+        <v>216</v>
+      </c>
+      <c r="C58" s="1">
         <v>11992874194</v>
       </c>
       <c r="D58" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E58" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="F58" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
     </row>
     <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B59" t="s">
-        <v>226</v>
-      </c>
-      <c r="C59">
+        <v>221</v>
+      </c>
+      <c r="C59" s="1">
         <v>38992274890</v>
       </c>
       <c r="D59" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="E59" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="F59" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="G59" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H59" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
     </row>
     <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B60" t="s">
-        <v>164</v>
-      </c>
-      <c r="C60">
+        <v>162</v>
+      </c>
+      <c r="C60" s="1">
         <v>14991294599</v>
       </c>
       <c r="D60" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="E60" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="F60" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="H60" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
     </row>
     <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B61" t="s">
-        <v>235</v>
-      </c>
-      <c r="C61">
+        <v>230</v>
+      </c>
+      <c r="C61" s="1">
         <v>38992168882</v>
       </c>
       <c r="D61" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="E61" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
     </row>
     <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
+        <v>229</v>
+      </c>
+      <c r="B62" t="s">
+        <v>233</v>
+      </c>
+      <c r="D62" t="s">
         <v>234</v>
       </c>
-      <c r="B62" t="s">
-        <v>238</v>
-      </c>
-      <c r="D62" t="s">
-        <v>239</v>
-      </c>
       <c r="E62" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B63" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D63" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="E63" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="B64" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D64" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="E64" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="B65" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D65" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="E65" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="H65" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
     </row>
   </sheetData>

</xml_diff>